<commit_message>
Update DataProvider - TakeScreenshot - Recordvideo
</commit_message>
<xml_diff>
--- a/SeleniumTestNG_Parallel/src/test/resources/testdata/LoginData.xlsx
+++ b/SeleniumTestNG_Parallel/src/test/resources/testdata/LoginData.xlsx
@@ -3,22 +3,23 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SE_Java\Project\java_selenium\SeleniumTestNG_Parallel\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D77662E-E550-4D9E-9264-489A01B2EF3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9B287AF-E50A-4B5E-A362-B11073AD9E58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{283991F2-45DD-49CF-9C49-1980B082935A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{283991F2-45DD-49CF-9C49-1980B082935A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="LoginData" sheetId="3" r:id="rId1"/>
+    <sheet name="LoginSuccess" sheetId="1" r:id="rId2"/>
+    <sheet name="LoginFail" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
   <si>
     <t>email</t>
   </si>
@@ -59,13 +60,21 @@
   </si>
   <si>
     <t>ProjectManager</t>
+  </si>
+  <si>
+    <t>employee123@example.com</t>
+  </si>
+  <si>
+    <t>1234567</t>
+  </si>
+  <si>
+    <t>1234568</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -83,7 +92,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -92,9 +101,6 @@
     </fill>
     <fill>
       <patternFill patternType="none"/>
-    </fill>
-    <fill>
-      <patternFill/>
     </fill>
   </fills>
   <borders count="1">
@@ -110,30 +116,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -448,30 +437,86 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{196270C3-9EFE-42DA-A0D0-ADC53F4EE2B6}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:F1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{19993BE2-2018-4354-AA17-F3C28D1CD6A5}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{BD35DD6F-3BBF-4770-979E-E7FCA2CF47AE}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{18C840C6-BAFE-4104-AC9B-3C4A5A93557A}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46BEEE4F-2721-4564-AFAC-1E65776D9A63}">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="27.42578125"/>
-    <col min="2" max="2" customWidth="true" width="13.0"/>
+    <col min="1" max="1" width="27.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -479,13 +524,13 @@
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="0">
+      <c r="B2">
         <v>123456</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -493,13 +538,13 @@
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="0">
+      <c r="B3">
         <v>123456</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="D3" t="s">
         <v>7</v>
       </c>
     </row>
@@ -512,38 +557,38 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EE6764D-86B4-48A5-9CCA-C1A728EAB6F9}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="29.5703125"/>
+    <col min="1" max="1" width="29.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s" s="8">
+      <c r="C2" s="2" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>